<commit_message>
new data processing outputs
</commit_message>
<xml_diff>
--- a/data/04_model_input/grangers_matrix.xlsx
+++ b/data/04_model_input/grangers_matrix.xlsx
@@ -939,13 +939,13 @@
         <v>0.02</v>
       </c>
       <c r="S2">
-        <v>0.7718</v>
+        <v>0.7735</v>
       </c>
       <c r="T2">
         <v>0.2141</v>
       </c>
       <c r="U2">
-        <v>0.8636</v>
+        <v>0.8702</v>
       </c>
       <c r="V2">
         <v>0.0589</v>
@@ -957,7 +957,7 @@
         <v>0.1823</v>
       </c>
       <c r="Y2">
-        <v>0.1701</v>
+        <v>0.166</v>
       </c>
       <c r="Z2">
         <v>0.3045</v>
@@ -1029,7 +1029,7 @@
         <v>0.0448</v>
       </c>
       <c r="AW2">
-        <v>0.1557</v>
+        <v>0.1525</v>
       </c>
       <c r="AX2">
         <v>0.2094</v>
@@ -1112,13 +1112,13 @@
         <v>0.151</v>
       </c>
       <c r="S3">
-        <v>0.041</v>
+        <v>0.0413</v>
       </c>
       <c r="T3">
         <v>0.0027</v>
       </c>
       <c r="U3">
-        <v>0.09810000000000001</v>
+        <v>0.0963</v>
       </c>
       <c r="V3">
         <v>0.4041</v>
@@ -1130,7 +1130,7 @@
         <v>0.0622</v>
       </c>
       <c r="Y3">
-        <v>0.3017</v>
+        <v>0.3024</v>
       </c>
       <c r="Z3">
         <v>0.0485</v>
@@ -1202,7 +1202,7 @@
         <v>0.3694</v>
       </c>
       <c r="AW3">
-        <v>0.0432</v>
+        <v>0.0463</v>
       </c>
       <c r="AX3">
         <v>0.3332</v>
@@ -1285,13 +1285,13 @@
         <v>0.0404</v>
       </c>
       <c r="S4">
-        <v>0.5518</v>
+        <v>0.5515</v>
       </c>
       <c r="T4">
         <v>0.272</v>
       </c>
       <c r="U4">
-        <v>0.4583</v>
+        <v>0.4752</v>
       </c>
       <c r="V4">
         <v>0.0275</v>
@@ -1303,7 +1303,7 @@
         <v>0.051</v>
       </c>
       <c r="Y4">
-        <v>0.0296</v>
+        <v>0.036</v>
       </c>
       <c r="Z4">
         <v>0.1608</v>
@@ -1375,7 +1375,7 @@
         <v>0.0955</v>
       </c>
       <c r="AW4">
-        <v>0.5518999999999999</v>
+        <v>0.5426</v>
       </c>
       <c r="AX4">
         <v>0.4777</v>
@@ -1458,13 +1458,13 @@
         <v>0.06619999999999999</v>
       </c>
       <c r="S5">
-        <v>0.2896</v>
+        <v>0.2897</v>
       </c>
       <c r="T5">
         <v>0.7664</v>
       </c>
       <c r="U5">
-        <v>0.1287</v>
+        <v>0.1044</v>
       </c>
       <c r="V5">
         <v>0</v>
@@ -1476,7 +1476,7 @@
         <v>0.2442</v>
       </c>
       <c r="Y5">
-        <v>0.0246</v>
+        <v>0.0218</v>
       </c>
       <c r="Z5">
         <v>0.1689</v>
@@ -1548,7 +1548,7 @@
         <v>0.6874</v>
       </c>
       <c r="AW5">
-        <v>0.2498</v>
+        <v>0.2433</v>
       </c>
       <c r="AX5">
         <v>0.7346</v>
@@ -1631,13 +1631,13 @@
         <v>0.7288</v>
       </c>
       <c r="S6">
-        <v>0.1734</v>
+        <v>0.174</v>
       </c>
       <c r="T6">
         <v>0.1874</v>
       </c>
       <c r="U6">
-        <v>0.2062</v>
+        <v>0.2097</v>
       </c>
       <c r="V6">
         <v>0.0071</v>
@@ -1649,7 +1649,7 @@
         <v>0.0334</v>
       </c>
       <c r="Y6">
-        <v>0.1313</v>
+        <v>0.1534</v>
       </c>
       <c r="Z6">
         <v>0.5211</v>
@@ -1721,7 +1721,7 @@
         <v>0.7586000000000001</v>
       </c>
       <c r="AW6">
-        <v>0.6911</v>
+        <v>0.6889</v>
       </c>
       <c r="AX6">
         <v>0.1759</v>
@@ -1804,13 +1804,13 @@
         <v>0.0021</v>
       </c>
       <c r="S7">
-        <v>0.2438</v>
+        <v>0.2446</v>
       </c>
       <c r="T7">
         <v>0.2014</v>
       </c>
       <c r="U7">
-        <v>0.1144</v>
+        <v>0.1014</v>
       </c>
       <c r="V7">
         <v>0.1672</v>
@@ -1822,7 +1822,7 @@
         <v>0.06950000000000001</v>
       </c>
       <c r="Y7">
-        <v>0.1213</v>
+        <v>0.1221</v>
       </c>
       <c r="Z7">
         <v>0.1645</v>
@@ -1894,7 +1894,7 @@
         <v>0.2958</v>
       </c>
       <c r="AW7">
-        <v>0.0228</v>
+        <v>0.0241</v>
       </c>
       <c r="AX7">
         <v>0.0033</v>
@@ -1977,13 +1977,13 @@
         <v>0.0069</v>
       </c>
       <c r="S8">
-        <v>0.125</v>
+        <v>0.126</v>
       </c>
       <c r="T8">
         <v>0.406</v>
       </c>
       <c r="U8">
-        <v>0.0146</v>
+        <v>0.0104</v>
       </c>
       <c r="V8">
         <v>0.0283</v>
@@ -2067,7 +2067,7 @@
         <v>0.0301</v>
       </c>
       <c r="AW8">
-        <v>0.3106</v>
+        <v>0.3338</v>
       </c>
       <c r="AX8">
         <v>0.0004</v>
@@ -2150,7 +2150,7 @@
         <v>0.0001</v>
       </c>
       <c r="S9">
-        <v>0.4412</v>
+        <v>0.4409</v>
       </c>
       <c r="T9">
         <v>0.3245</v>
@@ -2240,7 +2240,7 @@
         <v>0.0716</v>
       </c>
       <c r="AW9">
-        <v>0.1514</v>
+        <v>0.1496</v>
       </c>
       <c r="AX9">
         <v>0.0033</v>
@@ -2323,7 +2323,7 @@
         <v>0</v>
       </c>
       <c r="S10">
-        <v>0.2029</v>
+        <v>0.2034</v>
       </c>
       <c r="T10">
         <v>0.5623</v>
@@ -2413,7 +2413,7 @@
         <v>0.0609</v>
       </c>
       <c r="AW10">
-        <v>0.0412</v>
+        <v>0.0416</v>
       </c>
       <c r="AX10">
         <v>0.0448</v>
@@ -2496,13 +2496,13 @@
         <v>0</v>
       </c>
       <c r="S11">
-        <v>0.4488</v>
+        <v>0.4455</v>
       </c>
       <c r="T11">
         <v>0.5618</v>
       </c>
       <c r="U11">
-        <v>0.0837</v>
+        <v>0.08019999999999999</v>
       </c>
       <c r="V11">
         <v>0.2119</v>
@@ -2586,7 +2586,7 @@
         <v>0.0849</v>
       </c>
       <c r="AW11">
-        <v>0.5213</v>
+        <v>0.5493</v>
       </c>
       <c r="AX11">
         <v>0.4104</v>
@@ -2669,7 +2669,7 @@
         <v>0.0008</v>
       </c>
       <c r="S12">
-        <v>0.0245</v>
+        <v>0.0251</v>
       </c>
       <c r="T12">
         <v>0.1859</v>
@@ -2759,7 +2759,7 @@
         <v>0.0012</v>
       </c>
       <c r="AW12">
-        <v>0.188</v>
+        <v>0.1991</v>
       </c>
       <c r="AX12">
         <v>0.0014</v>
@@ -2842,13 +2842,13 @@
         <v>0.0001</v>
       </c>
       <c r="S13">
-        <v>0.6654</v>
+        <v>0.664</v>
       </c>
       <c r="T13">
         <v>0.4746</v>
       </c>
       <c r="U13">
-        <v>0.0446</v>
+        <v>0.052</v>
       </c>
       <c r="V13">
         <v>0.0321</v>
@@ -2932,7 +2932,7 @@
         <v>0.039</v>
       </c>
       <c r="AW13">
-        <v>0.3289</v>
+        <v>0.3176</v>
       </c>
       <c r="AX13">
         <v>0.591</v>
@@ -3015,13 +3015,13 @@
         <v>0.0183</v>
       </c>
       <c r="S14">
-        <v>0.4098</v>
+        <v>0.4113</v>
       </c>
       <c r="T14">
         <v>0.4873</v>
       </c>
       <c r="U14">
-        <v>0.2075</v>
+        <v>0.2094</v>
       </c>
       <c r="V14">
         <v>0.0173</v>
@@ -3033,7 +3033,7 @@
         <v>0.0728</v>
       </c>
       <c r="Y14">
-        <v>0.622</v>
+        <v>0.6225000000000001</v>
       </c>
       <c r="Z14">
         <v>0.7313</v>
@@ -3105,7 +3105,7 @@
         <v>0.5354</v>
       </c>
       <c r="AW14">
-        <v>0.5867</v>
+        <v>0.6102</v>
       </c>
       <c r="AX14">
         <v>0.1988</v>
@@ -3188,13 +3188,13 @@
         <v>0</v>
       </c>
       <c r="S15">
-        <v>0.0221</v>
+        <v>0.0222</v>
       </c>
       <c r="T15">
         <v>0.5308</v>
       </c>
       <c r="U15">
-        <v>0.0056</v>
+        <v>0.0054</v>
       </c>
       <c r="V15">
         <v>0</v>
@@ -3278,7 +3278,7 @@
         <v>0.3127</v>
       </c>
       <c r="AW15">
-        <v>0.1019</v>
+        <v>0.098</v>
       </c>
       <c r="AX15">
         <v>0.0786</v>
@@ -3361,13 +3361,13 @@
         <v>0</v>
       </c>
       <c r="S16">
-        <v>0.0014</v>
+        <v>0.0015</v>
       </c>
       <c r="T16">
         <v>0.1038</v>
       </c>
       <c r="U16">
-        <v>0.0057</v>
+        <v>0.006</v>
       </c>
       <c r="V16">
         <v>0.0134</v>
@@ -3451,7 +3451,7 @@
         <v>0.179</v>
       </c>
       <c r="AW16">
-        <v>0.2441</v>
+        <v>0.2458</v>
       </c>
       <c r="AX16">
         <v>0.254</v>
@@ -3534,13 +3534,13 @@
         <v>0.3816</v>
       </c>
       <c r="S17">
-        <v>0.0351</v>
+        <v>0.0352</v>
       </c>
       <c r="T17">
         <v>0.0104</v>
       </c>
       <c r="U17">
-        <v>0.0021</v>
+        <v>0.0023</v>
       </c>
       <c r="V17">
         <v>0.2481</v>
@@ -3552,7 +3552,7 @@
         <v>0.0038</v>
       </c>
       <c r="Y17">
-        <v>0.2165</v>
+        <v>0.2175</v>
       </c>
       <c r="Z17">
         <v>0.083</v>
@@ -3624,7 +3624,7 @@
         <v>0.0283</v>
       </c>
       <c r="AW17">
-        <v>0.3982</v>
+        <v>0.3893</v>
       </c>
       <c r="AX17">
         <v>0.1445</v>
@@ -3707,13 +3707,13 @@
         <v>1</v>
       </c>
       <c r="S18">
-        <v>0.4988</v>
+        <v>0.4999</v>
       </c>
       <c r="T18">
         <v>0.1903</v>
       </c>
       <c r="U18">
-        <v>0.1547</v>
+        <v>0.1521</v>
       </c>
       <c r="V18">
         <v>0.0038</v>
@@ -3725,7 +3725,7 @@
         <v>0.419</v>
       </c>
       <c r="Y18">
-        <v>0.036</v>
+        <v>0.0296</v>
       </c>
       <c r="Z18">
         <v>0.1431</v>
@@ -3797,7 +3797,7 @@
         <v>0.3344</v>
       </c>
       <c r="AW18">
-        <v>0.295</v>
+        <v>0.3069</v>
       </c>
       <c r="AX18">
         <v>0.2867</v>
@@ -3829,37 +3829,37 @@
         <v>73</v>
       </c>
       <c r="B19">
-        <v>0.2449</v>
+        <v>0.2448</v>
       </c>
       <c r="C19">
-        <v>0.0027</v>
+        <v>0.0028</v>
       </c>
       <c r="D19">
-        <v>0.0646</v>
+        <v>0.0648</v>
       </c>
       <c r="E19">
-        <v>0.0012</v>
+        <v>0.0013</v>
       </c>
       <c r="F19">
-        <v>0.0097</v>
+        <v>0.009599999999999999</v>
       </c>
       <c r="G19">
         <v>0.0001</v>
       </c>
       <c r="H19">
-        <v>0.094</v>
+        <v>0.09370000000000001</v>
       </c>
       <c r="I19">
-        <v>0.0601</v>
+        <v>0.0599</v>
       </c>
       <c r="J19">
-        <v>0.0466</v>
+        <v>0.0464</v>
       </c>
       <c r="K19">
         <v>0.0001</v>
       </c>
       <c r="L19">
-        <v>0.481</v>
+        <v>0.482</v>
       </c>
       <c r="M19">
         <v>0.0016</v>
@@ -3874,7 +3874,7 @@
         <v>0.0047</v>
       </c>
       <c r="Q19">
-        <v>0.1097</v>
+        <v>0.1091</v>
       </c>
       <c r="R19">
         <v>0.0038</v>
@@ -3883,40 +3883,40 @@
         <v>1</v>
       </c>
       <c r="T19">
-        <v>0.2276</v>
+        <v>0.2282</v>
       </c>
       <c r="U19">
-        <v>0.0344</v>
+        <v>0.039</v>
       </c>
       <c r="V19">
-        <v>0.0095</v>
+        <v>0.009599999999999999</v>
       </c>
       <c r="W19">
-        <v>0.6099</v>
+        <v>0.6101</v>
       </c>
       <c r="X19">
-        <v>0.0257</v>
+        <v>0.0259</v>
       </c>
       <c r="Y19">
-        <v>0.0116</v>
+        <v>0.0124</v>
       </c>
       <c r="Z19">
         <v>0.0098</v>
       </c>
       <c r="AA19">
-        <v>0.102</v>
+        <v>0.1025</v>
       </c>
       <c r="AB19">
         <v>0.0026</v>
       </c>
       <c r="AC19">
-        <v>0.043</v>
+        <v>0.0428</v>
       </c>
       <c r="AD19">
         <v>0.0001</v>
       </c>
       <c r="AE19">
-        <v>0.6514</v>
+        <v>0.648</v>
       </c>
       <c r="AF19">
         <v>0.0806</v>
@@ -3925,31 +3925,31 @@
         <v>0.0028</v>
       </c>
       <c r="AH19">
-        <v>0.0132</v>
+        <v>0.0131</v>
       </c>
       <c r="AI19">
         <v>0.0033</v>
       </c>
       <c r="AJ19">
-        <v>0.1343</v>
+        <v>0.134</v>
       </c>
       <c r="AK19">
-        <v>0.3981</v>
+        <v>0.3974</v>
       </c>
       <c r="AL19">
-        <v>0.1081</v>
+        <v>0.1065</v>
       </c>
       <c r="AM19">
-        <v>0.0149</v>
+        <v>0.015</v>
       </c>
       <c r="AN19">
         <v>0.0002</v>
       </c>
       <c r="AO19">
-        <v>0.2172</v>
+        <v>0.2181</v>
       </c>
       <c r="AP19">
-        <v>0.1952</v>
+        <v>0.1958</v>
       </c>
       <c r="AQ19">
         <v>0.0012</v>
@@ -3964,37 +3964,37 @@
         <v>0</v>
       </c>
       <c r="AU19">
-        <v>0.0297</v>
+        <v>0.03</v>
       </c>
       <c r="AV19">
-        <v>0.1723</v>
+        <v>0.1727</v>
       </c>
       <c r="AW19">
-        <v>0.6525</v>
+        <v>0.6663</v>
       </c>
       <c r="AX19">
-        <v>0.2918</v>
+        <v>0.2999</v>
       </c>
       <c r="AY19">
-        <v>0.3484</v>
+        <v>0.3468</v>
       </c>
       <c r="AZ19">
-        <v>0.4277</v>
+        <v>0.4257</v>
       </c>
       <c r="BA19">
-        <v>0.1351</v>
+        <v>0.1341</v>
       </c>
       <c r="BB19">
-        <v>0.1034</v>
+        <v>0.1053</v>
       </c>
       <c r="BC19">
         <v>0</v>
       </c>
       <c r="BD19">
-        <v>0.0216</v>
+        <v>0.0218</v>
       </c>
       <c r="BE19">
-        <v>0.0281</v>
+        <v>0.0282</v>
       </c>
     </row>
     <row r="20" spans="1:57">
@@ -4053,13 +4053,13 @@
         <v>0.3858</v>
       </c>
       <c r="S20">
-        <v>0.5534</v>
+        <v>0.552</v>
       </c>
       <c r="T20">
         <v>1</v>
       </c>
       <c r="U20">
-        <v>0.1841</v>
+        <v>0.1695</v>
       </c>
       <c r="V20">
         <v>0.7638</v>
@@ -4071,7 +4071,7 @@
         <v>0.4295</v>
       </c>
       <c r="Y20">
-        <v>0.4079</v>
+        <v>0.4162</v>
       </c>
       <c r="Z20">
         <v>0.2716</v>
@@ -4143,7 +4143,7 @@
         <v>0.0455</v>
       </c>
       <c r="AW20">
-        <v>0.0008</v>
+        <v>0.001</v>
       </c>
       <c r="AX20">
         <v>0.0473</v>
@@ -4175,172 +4175,172 @@
         <v>75</v>
       </c>
       <c r="B21">
-        <v>0.0135</v>
+        <v>0.014</v>
       </c>
       <c r="C21">
-        <v>0.0383</v>
+        <v>0.0483</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="E21">
-        <v>0.009299999999999999</v>
+        <v>0.0094</v>
       </c>
       <c r="F21">
-        <v>0.0343</v>
+        <v>0.0342</v>
       </c>
       <c r="G21">
-        <v>0.2659</v>
+        <v>0.28</v>
       </c>
       <c r="H21">
-        <v>0.6236</v>
+        <v>0.6477000000000001</v>
       </c>
       <c r="I21">
-        <v>0.2741</v>
+        <v>0.2927</v>
       </c>
       <c r="J21">
-        <v>0.4231</v>
+        <v>0.4331</v>
       </c>
       <c r="K21">
-        <v>0.1053</v>
+        <v>0.1135</v>
       </c>
       <c r="L21">
-        <v>0.4901</v>
+        <v>0.5348000000000001</v>
       </c>
       <c r="M21">
-        <v>0.4167</v>
+        <v>0.4222</v>
       </c>
       <c r="N21">
-        <v>0.0478</v>
+        <v>0.0457</v>
       </c>
       <c r="O21">
-        <v>0.0312</v>
+        <v>0.0355</v>
       </c>
       <c r="P21">
-        <v>0.3743</v>
+        <v>0.3473</v>
       </c>
       <c r="Q21">
-        <v>0.3418</v>
+        <v>0.3359</v>
       </c>
       <c r="R21">
-        <v>0.0036</v>
+        <v>0.0038</v>
       </c>
       <c r="S21">
-        <v>0.3135</v>
+        <v>0.2774</v>
       </c>
       <c r="T21">
-        <v>0.0047</v>
+        <v>0.0043</v>
       </c>
       <c r="U21">
         <v>1</v>
       </c>
       <c r="V21">
-        <v>0.1623</v>
+        <v>0.1601</v>
       </c>
       <c r="W21">
-        <v>0.8294</v>
+        <v>0.8287</v>
       </c>
       <c r="X21">
-        <v>0.0378</v>
+        <v>0.038</v>
       </c>
       <c r="Y21">
-        <v>0.0304</v>
+        <v>0.0531</v>
       </c>
       <c r="Z21">
-        <v>0.1841</v>
+        <v>0.1858</v>
       </c>
       <c r="AA21">
         <v>0.0001</v>
       </c>
       <c r="AB21">
-        <v>0.4397</v>
+        <v>0.4514</v>
       </c>
       <c r="AC21">
-        <v>0.378</v>
+        <v>0.4224</v>
       </c>
       <c r="AD21">
-        <v>0.096</v>
+        <v>0.0975</v>
       </c>
       <c r="AE21">
-        <v>0.3018</v>
+        <v>0.3604</v>
       </c>
       <c r="AF21">
-        <v>0.1663</v>
+        <v>0.2067</v>
       </c>
       <c r="AG21">
-        <v>0.2749</v>
+        <v>0.2907</v>
       </c>
       <c r="AH21">
-        <v>0.0589</v>
+        <v>0.0522</v>
       </c>
       <c r="AI21">
-        <v>0.551</v>
+        <v>0.5639999999999999</v>
       </c>
       <c r="AJ21">
-        <v>0.2495</v>
+        <v>0.2481</v>
       </c>
       <c r="AK21">
-        <v>0.1772</v>
+        <v>0.1729</v>
       </c>
       <c r="AL21">
-        <v>0.0018</v>
+        <v>0.0008</v>
       </c>
       <c r="AM21">
         <v>0.0005</v>
       </c>
       <c r="AN21">
-        <v>0.0396</v>
+        <v>0.0322</v>
       </c>
       <c r="AO21">
-        <v>0.5387999999999999</v>
+        <v>0.4953</v>
       </c>
       <c r="AP21">
-        <v>0.083</v>
+        <v>0.08989999999999999</v>
       </c>
       <c r="AQ21">
-        <v>0.0109</v>
+        <v>0.0115</v>
       </c>
       <c r="AR21">
-        <v>0.1561</v>
+        <v>0.1453</v>
       </c>
       <c r="AS21">
-        <v>0.0372</v>
+        <v>0.0417</v>
       </c>
       <c r="AT21">
-        <v>0.6544</v>
+        <v>0.644</v>
       </c>
       <c r="AU21">
-        <v>0.0528</v>
+        <v>0.0514</v>
       </c>
       <c r="AV21">
-        <v>0.0467</v>
+        <v>0.0451</v>
       </c>
       <c r="AW21">
-        <v>0.0554</v>
+        <v>0.06900000000000001</v>
       </c>
       <c r="AX21">
-        <v>0.2472</v>
+        <v>0.2463</v>
       </c>
       <c r="AY21">
-        <v>0.1606</v>
+        <v>0.2236</v>
       </c>
       <c r="AZ21">
-        <v>0.0694</v>
+        <v>0.1063</v>
       </c>
       <c r="BA21">
-        <v>0.3176</v>
+        <v>0.3095</v>
       </c>
       <c r="BB21">
-        <v>0.2152</v>
+        <v>0.2014</v>
       </c>
       <c r="BC21">
         <v>0.0016</v>
       </c>
       <c r="BD21">
-        <v>0.1248</v>
+        <v>0.1213</v>
       </c>
       <c r="BE21">
-        <v>0.1186</v>
+        <v>0.1104</v>
       </c>
     </row>
     <row r="22" spans="1:57">
@@ -4399,7 +4399,7 @@
         <v>0.0001</v>
       </c>
       <c r="S22">
-        <v>0.1965</v>
+        <v>0.198</v>
       </c>
       <c r="T22">
         <v>0.0189</v>
@@ -4489,7 +4489,7 @@
         <v>0.2812</v>
       </c>
       <c r="AW22">
-        <v>0.0699</v>
+        <v>0.0653</v>
       </c>
       <c r="AX22">
         <v>0.2112</v>
@@ -4572,13 +4572,13 @@
         <v>0.0057</v>
       </c>
       <c r="S23">
-        <v>0.0077</v>
+        <v>0.007900000000000001</v>
       </c>
       <c r="T23">
         <v>0.389</v>
       </c>
       <c r="U23">
-        <v>0.0185</v>
+        <v>0.0192</v>
       </c>
       <c r="V23">
         <v>0.0003</v>
@@ -4590,7 +4590,7 @@
         <v>0.0055</v>
       </c>
       <c r="Y23">
-        <v>0.0029</v>
+        <v>0.0028</v>
       </c>
       <c r="Z23">
         <v>0.0049</v>
@@ -4662,7 +4662,7 @@
         <v>0.0075</v>
       </c>
       <c r="AW23">
-        <v>0.4195</v>
+        <v>0.413</v>
       </c>
       <c r="AX23">
         <v>0.2421</v>
@@ -4745,13 +4745,13 @@
         <v>0.0025</v>
       </c>
       <c r="S24">
-        <v>0.3471</v>
+        <v>0.3475</v>
       </c>
       <c r="T24">
         <v>0.2607</v>
       </c>
       <c r="U24">
-        <v>0.0605</v>
+        <v>0.0596</v>
       </c>
       <c r="V24">
         <v>0.08</v>
@@ -4763,7 +4763,7 @@
         <v>1</v>
       </c>
       <c r="Y24">
-        <v>0.0062</v>
+        <v>0.005</v>
       </c>
       <c r="Z24">
         <v>0.0317</v>
@@ -4835,7 +4835,7 @@
         <v>0.2196</v>
       </c>
       <c r="AW24">
-        <v>0.7309</v>
+        <v>0.7346</v>
       </c>
       <c r="AX24">
         <v>0.1716</v>
@@ -4867,49 +4867,49 @@
         <v>79</v>
       </c>
       <c r="B25">
-        <v>0.0266</v>
+        <v>0.0273</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25">
-        <v>0.0233</v>
+        <v>0.0259</v>
       </c>
       <c r="E25">
         <v>0.0002</v>
       </c>
       <c r="F25">
-        <v>0.0213</v>
+        <v>0.022</v>
       </c>
       <c r="G25">
-        <v>0.2702</v>
+        <v>0.2717</v>
       </c>
       <c r="H25">
-        <v>0.4782</v>
+        <v>0.4634</v>
       </c>
       <c r="I25">
-        <v>0.0798</v>
+        <v>0.08740000000000001</v>
       </c>
       <c r="J25">
-        <v>0.1485</v>
+        <v>0.1529</v>
       </c>
       <c r="K25">
-        <v>0.0061</v>
+        <v>0.0074</v>
       </c>
       <c r="L25">
-        <v>0.1947</v>
+        <v>0.1983</v>
       </c>
       <c r="M25">
-        <v>0.0561</v>
+        <v>0.0603</v>
       </c>
       <c r="N25">
         <v>0.0009</v>
       </c>
       <c r="O25">
-        <v>0.0057</v>
+        <v>0.0054</v>
       </c>
       <c r="P25">
-        <v>0.0775</v>
+        <v>0.07679999999999999</v>
       </c>
       <c r="Q25">
         <v>0.307</v>
@@ -4918,79 +4918,79 @@
         <v>0.0002</v>
       </c>
       <c r="S25">
-        <v>0.4596</v>
+        <v>0.4113</v>
       </c>
       <c r="T25">
-        <v>0.5108</v>
+        <v>0.5318000000000001</v>
       </c>
       <c r="U25">
-        <v>0.0042</v>
+        <v>0.0038</v>
       </c>
       <c r="V25">
-        <v>0.0698</v>
+        <v>0.0711</v>
       </c>
       <c r="W25">
-        <v>0.1127</v>
+        <v>0.1247</v>
       </c>
       <c r="X25">
-        <v>0.0201</v>
+        <v>0.0212</v>
       </c>
       <c r="Y25">
         <v>1</v>
       </c>
       <c r="Z25">
-        <v>0.008999999999999999</v>
+        <v>0.0113</v>
       </c>
       <c r="AA25">
-        <v>0.6138</v>
+        <v>0.6006</v>
       </c>
       <c r="AB25">
-        <v>0.1362</v>
+        <v>0.1397</v>
       </c>
       <c r="AC25">
-        <v>0.6514</v>
+        <v>0.6636</v>
       </c>
       <c r="AD25">
-        <v>0.1756</v>
+        <v>0.1888</v>
       </c>
       <c r="AE25">
-        <v>0.5645</v>
+        <v>0.5775</v>
       </c>
       <c r="AF25">
-        <v>0.0199</v>
+        <v>0.0209</v>
       </c>
       <c r="AG25">
-        <v>0.0526</v>
+        <v>0.055</v>
       </c>
       <c r="AH25">
-        <v>0.0119</v>
+        <v>0.0125</v>
       </c>
       <c r="AI25">
-        <v>0.0629</v>
+        <v>0.06469999999999999</v>
       </c>
       <c r="AJ25">
-        <v>0.4163</v>
+        <v>0.4164</v>
       </c>
       <c r="AK25">
-        <v>0.1618</v>
+        <v>0.1661</v>
       </c>
       <c r="AL25">
-        <v>0.5344</v>
+        <v>0.5048</v>
       </c>
       <c r="AM25">
-        <v>0.0505</v>
+        <v>0.0546</v>
       </c>
       <c r="AN25">
-        <v>0.2762</v>
+        <v>0.2825</v>
       </c>
       <c r="AO25">
-        <v>0.2739</v>
+        <v>0.2699</v>
       </c>
       <c r="AP25">
-        <v>0.1943</v>
+        <v>0.2116</v>
       </c>
       <c r="AQ25">
-        <v>0.0127</v>
+        <v>0.0135</v>
       </c>
       <c r="AR25">
         <v>0.0003</v>
@@ -4999,40 +4999,40 @@
         <v>0</v>
       </c>
       <c r="AT25">
-        <v>0.0107</v>
+        <v>0.0118</v>
       </c>
       <c r="AU25">
-        <v>0.0153</v>
+        <v>0.0149</v>
       </c>
       <c r="AV25">
-        <v>0.4869</v>
+        <v>0.4996</v>
       </c>
       <c r="AW25">
-        <v>0.0588</v>
+        <v>0.0697</v>
       </c>
       <c r="AX25">
-        <v>0.393</v>
+        <v>0.3991</v>
       </c>
       <c r="AY25">
-        <v>0.4036</v>
+        <v>0.4297</v>
       </c>
       <c r="AZ25">
-        <v>0.4434</v>
+        <v>0.4442</v>
       </c>
       <c r="BA25">
-        <v>0.7839</v>
+        <v>0.7976</v>
       </c>
       <c r="BB25">
-        <v>0.0508</v>
+        <v>0.0456</v>
       </c>
       <c r="BC25">
-        <v>0.0008</v>
+        <v>0.001</v>
       </c>
       <c r="BD25">
         <v>0.0017</v>
       </c>
       <c r="BE25">
-        <v>0.0089</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="26" spans="1:57">
@@ -5091,13 +5091,13 @@
         <v>0.0014</v>
       </c>
       <c r="S26">
-        <v>0.0268</v>
+        <v>0.0272</v>
       </c>
       <c r="T26">
         <v>0.169</v>
       </c>
       <c r="U26">
-        <v>0.0013</v>
+        <v>0.0005999999999999999</v>
       </c>
       <c r="V26">
         <v>0.0007</v>
@@ -5181,7 +5181,7 @@
         <v>0.6349</v>
       </c>
       <c r="AW26">
-        <v>0.1</v>
+        <v>0.09959999999999999</v>
       </c>
       <c r="AX26">
         <v>0.2734</v>
@@ -5264,13 +5264,13 @@
         <v>0.0023</v>
       </c>
       <c r="S27">
-        <v>0.218</v>
+        <v>0.2177</v>
       </c>
       <c r="T27">
         <v>0.1399</v>
       </c>
       <c r="U27">
-        <v>0.0341</v>
+        <v>0.0352</v>
       </c>
       <c r="V27">
         <v>0.0013</v>
@@ -5354,7 +5354,7 @@
         <v>0.0585</v>
       </c>
       <c r="AW27">
-        <v>0.1213</v>
+        <v>0.1328</v>
       </c>
       <c r="AX27">
         <v>0.0318</v>
@@ -5443,7 +5443,7 @@
         <v>0.3586</v>
       </c>
       <c r="U28">
-        <v>0.0543</v>
+        <v>0.0462</v>
       </c>
       <c r="V28">
         <v>0.2259</v>
@@ -5527,7 +5527,7 @@
         <v>0.3299</v>
       </c>
       <c r="AW28">
-        <v>0.0048</v>
+        <v>0.0057</v>
       </c>
       <c r="AX28">
         <v>0.6059</v>
@@ -5610,13 +5610,13 @@
         <v>0</v>
       </c>
       <c r="S29">
-        <v>0.0851</v>
+        <v>0.0847</v>
       </c>
       <c r="T29">
         <v>0.463</v>
       </c>
       <c r="U29">
-        <v>0.0005999999999999999</v>
+        <v>0.0005</v>
       </c>
       <c r="V29">
         <v>0.0069</v>
@@ -5700,7 +5700,7 @@
         <v>0.2673</v>
       </c>
       <c r="AW29">
-        <v>0.1416</v>
+        <v>0.1393</v>
       </c>
       <c r="AX29">
         <v>0.0073</v>
@@ -5783,13 +5783,13 @@
         <v>0.089</v>
       </c>
       <c r="S30">
-        <v>0.515</v>
+        <v>0.5175999999999999</v>
       </c>
       <c r="T30">
         <v>0.2434</v>
       </c>
       <c r="U30">
-        <v>0.1881</v>
+        <v>0.1904</v>
       </c>
       <c r="V30">
         <v>0.4212</v>
@@ -5801,7 +5801,7 @@
         <v>0.3897</v>
       </c>
       <c r="Y30">
-        <v>0.0588</v>
+        <v>0.062</v>
       </c>
       <c r="Z30">
         <v>0.1892</v>
@@ -5873,7 +5873,7 @@
         <v>0.336</v>
       </c>
       <c r="AW30">
-        <v>0.1505</v>
+        <v>0.1559</v>
       </c>
       <c r="AX30">
         <v>0.0106</v>
@@ -5956,7 +5956,7 @@
         <v>0.0075</v>
       </c>
       <c r="S31">
-        <v>0.4871</v>
+        <v>0.4859</v>
       </c>
       <c r="T31">
         <v>0.0596</v>
@@ -6046,7 +6046,7 @@
         <v>0.1252</v>
       </c>
       <c r="AW31">
-        <v>0.3065</v>
+        <v>0.3272</v>
       </c>
       <c r="AX31">
         <v>0.164</v>
@@ -6129,7 +6129,7 @@
         <v>0.007</v>
       </c>
       <c r="S32">
-        <v>0.5919</v>
+        <v>0.5921999999999999</v>
       </c>
       <c r="T32">
         <v>0.0012</v>
@@ -6147,7 +6147,7 @@
         <v>0.1374</v>
       </c>
       <c r="Y32">
-        <v>0.0333</v>
+        <v>0.0357</v>
       </c>
       <c r="Z32">
         <v>0.5825</v>
@@ -6219,7 +6219,7 @@
         <v>0.2679</v>
       </c>
       <c r="AW32">
-        <v>0.0021</v>
+        <v>0.0026</v>
       </c>
       <c r="AX32">
         <v>0.0004</v>
@@ -6302,7 +6302,7 @@
         <v>0.0007</v>
       </c>
       <c r="S33">
-        <v>0.008699999999999999</v>
+        <v>0.0089</v>
       </c>
       <c r="T33">
         <v>0.1728</v>
@@ -6392,7 +6392,7 @@
         <v>0</v>
       </c>
       <c r="AW33">
-        <v>0.0119</v>
+        <v>0.0126</v>
       </c>
       <c r="AX33">
         <v>0.002</v>
@@ -6475,13 +6475,13 @@
         <v>0.3706</v>
       </c>
       <c r="S34">
-        <v>0.1228</v>
+        <v>0.123</v>
       </c>
       <c r="T34">
         <v>0.0655</v>
       </c>
       <c r="U34">
-        <v>0.049</v>
+        <v>0.0509</v>
       </c>
       <c r="V34">
         <v>0.0123</v>
@@ -6493,7 +6493,7 @@
         <v>0.0478</v>
       </c>
       <c r="Y34">
-        <v>0.0453</v>
+        <v>0.05</v>
       </c>
       <c r="Z34">
         <v>0.052</v>
@@ -6565,7 +6565,7 @@
         <v>0.0197</v>
       </c>
       <c r="AW34">
-        <v>0.1184</v>
+        <v>0.125</v>
       </c>
       <c r="AX34">
         <v>0.0041</v>
@@ -6648,13 +6648,13 @@
         <v>0.0003</v>
       </c>
       <c r="S35">
-        <v>0.0187</v>
+        <v>0.019</v>
       </c>
       <c r="T35">
         <v>0.1455</v>
       </c>
       <c r="U35">
-        <v>0.0043</v>
+        <v>0.0041</v>
       </c>
       <c r="V35">
         <v>0.0116</v>
@@ -6738,7 +6738,7 @@
         <v>0.4795</v>
       </c>
       <c r="AW35">
-        <v>0.1969</v>
+        <v>0.2009</v>
       </c>
       <c r="AX35">
         <v>0.7509</v>
@@ -6821,13 +6821,13 @@
         <v>0.0008</v>
       </c>
       <c r="S36">
-        <v>0.0094</v>
+        <v>0.0095</v>
       </c>
       <c r="T36">
         <v>0.2122</v>
       </c>
       <c r="U36">
-        <v>0.0012</v>
+        <v>0.0011</v>
       </c>
       <c r="V36">
         <v>0.0002</v>
@@ -6911,7 +6911,7 @@
         <v>0.0014</v>
       </c>
       <c r="AW36">
-        <v>0.1255</v>
+        <v>0.1322</v>
       </c>
       <c r="AX36">
         <v>0.0253</v>
@@ -6994,7 +6994,7 @@
         <v>0.0007</v>
       </c>
       <c r="S37">
-        <v>0.0155</v>
+        <v>0.0156</v>
       </c>
       <c r="T37">
         <v>0.2704</v>
@@ -7084,7 +7084,7 @@
         <v>0.0007</v>
       </c>
       <c r="AW37">
-        <v>0.1237</v>
+        <v>0.1297</v>
       </c>
       <c r="AX37">
         <v>0.0213</v>
@@ -7167,13 +7167,13 @@
         <v>0.2627</v>
       </c>
       <c r="S38">
-        <v>0.3773</v>
+        <v>0.3802</v>
       </c>
       <c r="T38">
         <v>0.1722</v>
       </c>
       <c r="U38">
-        <v>0.0868</v>
+        <v>0.0948</v>
       </c>
       <c r="V38">
         <v>0.2776</v>
@@ -7185,7 +7185,7 @@
         <v>0.1293</v>
       </c>
       <c r="Y38">
-        <v>0.0741</v>
+        <v>0.08699999999999999</v>
       </c>
       <c r="Z38">
         <v>0.0013</v>
@@ -7257,7 +7257,7 @@
         <v>0.1599</v>
       </c>
       <c r="AW38">
-        <v>0.3229</v>
+        <v>0.288</v>
       </c>
       <c r="AX38">
         <v>0.1783</v>
@@ -7346,7 +7346,7 @@
         <v>0.0522</v>
       </c>
       <c r="U39">
-        <v>0.3039</v>
+        <v>0.3326</v>
       </c>
       <c r="V39">
         <v>0.2015</v>
@@ -7358,7 +7358,7 @@
         <v>0.2079</v>
       </c>
       <c r="Y39">
-        <v>0.0795</v>
+        <v>0.0776</v>
       </c>
       <c r="Z39">
         <v>0.0235</v>
@@ -7430,7 +7430,7 @@
         <v>0.6834</v>
       </c>
       <c r="AW39">
-        <v>0.2582</v>
+        <v>0.2438</v>
       </c>
       <c r="AX39">
         <v>0.007</v>
@@ -7513,13 +7513,13 @@
         <v>0.0024</v>
       </c>
       <c r="S40">
-        <v>0.1041</v>
+        <v>0.1056</v>
       </c>
       <c r="T40">
         <v>0.0056</v>
       </c>
       <c r="U40">
-        <v>0.0148</v>
+        <v>0.0153</v>
       </c>
       <c r="V40">
         <v>0.0307</v>
@@ -7603,7 +7603,7 @@
         <v>0.8793</v>
       </c>
       <c r="AW40">
-        <v>0.027</v>
+        <v>0.0266</v>
       </c>
       <c r="AX40">
         <v>0.219</v>
@@ -7686,13 +7686,13 @@
         <v>0.002</v>
       </c>
       <c r="S41">
-        <v>0.2283</v>
+        <v>0.2291</v>
       </c>
       <c r="T41">
         <v>0.6471</v>
       </c>
       <c r="U41">
-        <v>0.008500000000000001</v>
+        <v>0.0068</v>
       </c>
       <c r="V41">
         <v>0.0298</v>
@@ -7776,7 +7776,7 @@
         <v>0.056</v>
       </c>
       <c r="AW41">
-        <v>0.2139</v>
+        <v>0.2192</v>
       </c>
       <c r="AX41">
         <v>0.0253</v>
@@ -7859,7 +7859,7 @@
         <v>0.0012</v>
       </c>
       <c r="S42">
-        <v>0.0174</v>
+        <v>0.0175</v>
       </c>
       <c r="T42">
         <v>0.0703</v>
@@ -7877,7 +7877,7 @@
         <v>0.074</v>
       </c>
       <c r="Y42">
-        <v>0.0106</v>
+        <v>0.0108</v>
       </c>
       <c r="Z42">
         <v>0.1771</v>
@@ -8032,7 +8032,7 @@
         <v>0</v>
       </c>
       <c r="S43">
-        <v>0.364</v>
+        <v>0.3644</v>
       </c>
       <c r="T43">
         <v>0.4381</v>
@@ -8205,13 +8205,13 @@
         <v>0.1334</v>
       </c>
       <c r="S44">
-        <v>0.1134</v>
+        <v>0.1148</v>
       </c>
       <c r="T44">
         <v>0.4556</v>
       </c>
       <c r="U44">
-        <v>0.0109</v>
+        <v>0.011</v>
       </c>
       <c r="V44">
         <v>0.0013</v>
@@ -8295,7 +8295,7 @@
         <v>0.0563</v>
       </c>
       <c r="AW44">
-        <v>0.0464</v>
+        <v>0.0466</v>
       </c>
       <c r="AX44">
         <v>0.062</v>
@@ -8378,13 +8378,13 @@
         <v>0.2205</v>
       </c>
       <c r="S45">
-        <v>0.0376</v>
+        <v>0.0374</v>
       </c>
       <c r="T45">
         <v>0.3302</v>
       </c>
       <c r="U45">
-        <v>0.1061</v>
+        <v>0.1109</v>
       </c>
       <c r="V45">
         <v>0.0019</v>
@@ -8396,7 +8396,7 @@
         <v>0.0241</v>
       </c>
       <c r="Y45">
-        <v>0.0009</v>
+        <v>0.0014</v>
       </c>
       <c r="Z45">
         <v>0.4376</v>
@@ -8468,7 +8468,7 @@
         <v>0.3267</v>
       </c>
       <c r="AW45">
-        <v>0.2587</v>
+        <v>0.2458</v>
       </c>
       <c r="AX45">
         <v>0.3033</v>
@@ -8557,7 +8557,7 @@
         <v>0.3002</v>
       </c>
       <c r="U46">
-        <v>0.0397</v>
+        <v>0.042</v>
       </c>
       <c r="V46">
         <v>0.021</v>
@@ -8569,7 +8569,7 @@
         <v>0.0011</v>
       </c>
       <c r="Y46">
-        <v>0.0256</v>
+        <v>0.0231</v>
       </c>
       <c r="Z46">
         <v>0.0273</v>
@@ -8641,7 +8641,7 @@
         <v>0.8653999999999999</v>
       </c>
       <c r="AW46">
-        <v>0.0999</v>
+        <v>0.09470000000000001</v>
       </c>
       <c r="AX46">
         <v>0.5145999999999999</v>
@@ -8724,7 +8724,7 @@
         <v>0.0069</v>
       </c>
       <c r="S47">
-        <v>0.2743</v>
+        <v>0.2751</v>
       </c>
       <c r="T47">
         <v>0.0045</v>
@@ -8742,7 +8742,7 @@
         <v>0.0061</v>
       </c>
       <c r="Y47">
-        <v>0.049</v>
+        <v>0.047</v>
       </c>
       <c r="Z47">
         <v>0.1107</v>
@@ -8897,13 +8897,13 @@
         <v>0</v>
       </c>
       <c r="S48">
-        <v>0.06320000000000001</v>
+        <v>0.0645</v>
       </c>
       <c r="T48">
         <v>0.0272</v>
       </c>
       <c r="U48">
-        <v>0.0018</v>
+        <v>0.0017</v>
       </c>
       <c r="V48">
         <v>0.0124</v>
@@ -8987,7 +8987,7 @@
         <v>1</v>
       </c>
       <c r="AW48">
-        <v>0.2041</v>
+        <v>0.2147</v>
       </c>
       <c r="AX48">
         <v>0.2523</v>
@@ -9019,43 +9019,43 @@
         <v>103</v>
       </c>
       <c r="B49">
-        <v>0.141</v>
+        <v>0.1392</v>
       </c>
       <c r="C49">
-        <v>0.0519</v>
+        <v>0.0529</v>
       </c>
       <c r="D49">
-        <v>0.3113</v>
+        <v>0.3116</v>
       </c>
       <c r="E49">
-        <v>0.0274</v>
+        <v>0.0264</v>
       </c>
       <c r="F49">
-        <v>0.7082000000000001</v>
+        <v>0.7088</v>
       </c>
       <c r="G49">
-        <v>0.1952</v>
+        <v>0.1954</v>
       </c>
       <c r="H49">
-        <v>0.2968</v>
+        <v>0.2902</v>
       </c>
       <c r="I49">
-        <v>0.1636</v>
+        <v>0.1645</v>
       </c>
       <c r="J49">
-        <v>0.022</v>
+        <v>0.0215</v>
       </c>
       <c r="K49">
-        <v>0.0204</v>
+        <v>0.0182</v>
       </c>
       <c r="L49">
-        <v>0.2568</v>
+        <v>0.2563</v>
       </c>
       <c r="M49">
-        <v>0.0303</v>
+        <v>0.0328</v>
       </c>
       <c r="N49">
-        <v>0.0192</v>
+        <v>0.02</v>
       </c>
       <c r="O49">
         <v>0.0001</v>
@@ -9064,79 +9064,79 @@
         <v>0.0005</v>
       </c>
       <c r="Q49">
-        <v>0.3096</v>
+        <v>0.3114</v>
       </c>
       <c r="R49">
-        <v>0.008999999999999999</v>
+        <v>0.0089</v>
       </c>
       <c r="S49">
-        <v>0.323</v>
+        <v>0.3087</v>
       </c>
       <c r="T49">
-        <v>0.2225</v>
+        <v>0.2193</v>
       </c>
       <c r="U49">
         <v>0.001</v>
       </c>
       <c r="V49">
-        <v>0.0508</v>
+        <v>0.0501</v>
       </c>
       <c r="W49">
-        <v>0.7203000000000001</v>
+        <v>0.7281</v>
       </c>
       <c r="X49">
-        <v>0.0706</v>
+        <v>0.0682</v>
       </c>
       <c r="Y49">
-        <v>0.0532</v>
+        <v>0.0457</v>
       </c>
       <c r="Z49">
-        <v>0.1463</v>
+        <v>0.1416</v>
       </c>
       <c r="AA49">
-        <v>0.1179</v>
+        <v>0.1218</v>
       </c>
       <c r="AB49">
-        <v>0.1361</v>
+        <v>0.141</v>
       </c>
       <c r="AC49">
-        <v>0.0075</v>
+        <v>0.0073</v>
       </c>
       <c r="AD49">
-        <v>0.1445</v>
+        <v>0.1426</v>
       </c>
       <c r="AE49">
-        <v>0.0078</v>
+        <v>0.008</v>
       </c>
       <c r="AF49">
-        <v>0.0271</v>
+        <v>0.0259</v>
       </c>
       <c r="AG49">
-        <v>0.0842</v>
+        <v>0.0813</v>
       </c>
       <c r="AH49">
-        <v>0.3073</v>
+        <v>0.3016</v>
       </c>
       <c r="AI49">
         <v>0.0003</v>
       </c>
       <c r="AJ49">
-        <v>0.4281</v>
+        <v>0.429</v>
       </c>
       <c r="AK49">
-        <v>0.4768</v>
+        <v>0.481</v>
       </c>
       <c r="AL49">
-        <v>0.1101</v>
+        <v>0.121</v>
       </c>
       <c r="AM49">
         <v>0.0009</v>
       </c>
       <c r="AN49">
-        <v>0.0102</v>
+        <v>0.0101</v>
       </c>
       <c r="AO49">
-        <v>0.3257</v>
+        <v>0.3203</v>
       </c>
       <c r="AP49">
         <v>0.0014</v>
@@ -9145,46 +9145,46 @@
         <v>0.0009</v>
       </c>
       <c r="AR49">
-        <v>0.4192</v>
+        <v>0.418</v>
       </c>
       <c r="AS49">
-        <v>0.08169999999999999</v>
+        <v>0.0862</v>
       </c>
       <c r="AT49">
-        <v>0.0857</v>
+        <v>0.0863</v>
       </c>
       <c r="AU49">
-        <v>0.0016</v>
+        <v>0.0017</v>
       </c>
       <c r="AV49">
-        <v>0.1273</v>
+        <v>0.1283</v>
       </c>
       <c r="AW49">
         <v>1</v>
       </c>
       <c r="AX49">
-        <v>0.7586000000000001</v>
+        <v>0.7514999999999999</v>
       </c>
       <c r="AY49">
-        <v>0.152</v>
+        <v>0.1537</v>
       </c>
       <c r="AZ49">
-        <v>0.2787</v>
+        <v>0.2803</v>
       </c>
       <c r="BA49">
-        <v>0.0053</v>
+        <v>0.0045</v>
       </c>
       <c r="BB49">
-        <v>0.2421</v>
+        <v>0.2473</v>
       </c>
       <c r="BC49">
-        <v>0.0176</v>
+        <v>0.0178</v>
       </c>
       <c r="BD49">
-        <v>0.1075</v>
+        <v>0.1071</v>
       </c>
       <c r="BE49">
-        <v>0.1147</v>
+        <v>0.1213</v>
       </c>
     </row>
     <row r="50" spans="1:57">
@@ -9243,13 +9243,13 @@
         <v>0.1062</v>
       </c>
       <c r="S50">
-        <v>0.1731</v>
+        <v>0.1768</v>
       </c>
       <c r="T50">
         <v>0.5003</v>
       </c>
       <c r="U50">
-        <v>0.1235</v>
+        <v>0.0979</v>
       </c>
       <c r="V50">
         <v>0.5253</v>
@@ -9261,7 +9261,7 @@
         <v>0.337</v>
       </c>
       <c r="Y50">
-        <v>0.0775</v>
+        <v>0.0752</v>
       </c>
       <c r="Z50">
         <v>0.0228</v>
@@ -9333,7 +9333,7 @@
         <v>0.2038</v>
       </c>
       <c r="AW50">
-        <v>0.2113</v>
+        <v>0.2009</v>
       </c>
       <c r="AX50">
         <v>1</v>
@@ -9416,13 +9416,13 @@
         <v>0.1304</v>
       </c>
       <c r="S51">
-        <v>0.1108</v>
+        <v>0.1088</v>
       </c>
       <c r="T51">
         <v>0.3439</v>
       </c>
       <c r="U51">
-        <v>0.0601</v>
+        <v>0.1001</v>
       </c>
       <c r="V51">
         <v>0.6722</v>
@@ -9434,7 +9434,7 @@
         <v>0.2699</v>
       </c>
       <c r="Y51">
-        <v>0.7398</v>
+        <v>0.7531</v>
       </c>
       <c r="Z51">
         <v>0.3277</v>
@@ -9506,7 +9506,7 @@
         <v>0.2092</v>
       </c>
       <c r="AW51">
-        <v>0.0494</v>
+        <v>0.0612</v>
       </c>
       <c r="AX51">
         <v>0.3354</v>
@@ -9589,13 +9589,13 @@
         <v>0.1712</v>
       </c>
       <c r="S52">
-        <v>0.3437</v>
+        <v>0.3394</v>
       </c>
       <c r="T52">
         <v>0.4709</v>
       </c>
       <c r="U52">
-        <v>0.3759</v>
+        <v>0.4103</v>
       </c>
       <c r="V52">
         <v>0.6844</v>
@@ -9607,7 +9607,7 @@
         <v>0.3529</v>
       </c>
       <c r="Y52">
-        <v>0.7237</v>
+        <v>0.7592</v>
       </c>
       <c r="Z52">
         <v>0.164</v>
@@ -9679,7 +9679,7 @@
         <v>0.1947</v>
       </c>
       <c r="AW52">
-        <v>0.1168</v>
+        <v>0.1409</v>
       </c>
       <c r="AX52">
         <v>0.1651</v>
@@ -9762,13 +9762,13 @@
         <v>0.475</v>
       </c>
       <c r="S53">
-        <v>0.768</v>
+        <v>0.7657</v>
       </c>
       <c r="T53">
         <v>0.4271</v>
       </c>
       <c r="U53">
-        <v>0.0262</v>
+        <v>0.0277</v>
       </c>
       <c r="V53">
         <v>0.1489</v>
@@ -9780,7 +9780,7 @@
         <v>0.2728</v>
       </c>
       <c r="Y53">
-        <v>0.238</v>
+        <v>0.2348</v>
       </c>
       <c r="Z53">
         <v>0.2606</v>
@@ -9852,7 +9852,7 @@
         <v>0.2776</v>
       </c>
       <c r="AW53">
-        <v>0.0005</v>
+        <v>0.0011</v>
       </c>
       <c r="AX53">
         <v>0.0442</v>
@@ -9935,13 +9935,13 @@
         <v>0.0547</v>
       </c>
       <c r="S54">
-        <v>0.7663</v>
+        <v>0.7714</v>
       </c>
       <c r="T54">
         <v>0.4315</v>
       </c>
       <c r="U54">
-        <v>0.5265</v>
+        <v>0.45</v>
       </c>
       <c r="V54">
         <v>0.0581</v>
@@ -9953,7 +9953,7 @@
         <v>0.3197</v>
       </c>
       <c r="Y54">
-        <v>0.0322</v>
+        <v>0.031</v>
       </c>
       <c r="Z54">
         <v>0.0622</v>
@@ -10025,7 +10025,7 @@
         <v>0.0863</v>
       </c>
       <c r="AW54">
-        <v>0.5967</v>
+        <v>0.5345</v>
       </c>
       <c r="AX54">
         <v>0.3064</v>
@@ -10108,13 +10108,13 @@
         <v>0.0047</v>
       </c>
       <c r="S55">
-        <v>0.2636</v>
+        <v>0.2603</v>
       </c>
       <c r="T55">
         <v>0.1876</v>
       </c>
       <c r="U55">
-        <v>0.0021</v>
+        <v>0.0016</v>
       </c>
       <c r="V55">
         <v>0.1158</v>
@@ -10126,7 +10126,7 @@
         <v>0.0452</v>
       </c>
       <c r="Y55">
-        <v>0.0138</v>
+        <v>0.0147</v>
       </c>
       <c r="Z55">
         <v>0.2311</v>
@@ -10198,7 +10198,7 @@
         <v>0.0397</v>
       </c>
       <c r="AW55">
-        <v>0.6015</v>
+        <v>0.5995</v>
       </c>
       <c r="AX55">
         <v>0.0021</v>
@@ -10281,13 +10281,13 @@
         <v>0.0306</v>
       </c>
       <c r="S56">
-        <v>0.3808</v>
+        <v>0.3822</v>
       </c>
       <c r="T56">
         <v>0.0155</v>
       </c>
       <c r="U56">
-        <v>0.0364</v>
+        <v>0.04</v>
       </c>
       <c r="V56">
         <v>0.227</v>
@@ -10299,7 +10299,7 @@
         <v>0.0898</v>
       </c>
       <c r="Y56">
-        <v>0.0498</v>
+        <v>0.0508</v>
       </c>
       <c r="Z56">
         <v>0.8111</v>
@@ -10371,7 +10371,7 @@
         <v>0.4935</v>
       </c>
       <c r="AW56">
-        <v>0.3058</v>
+        <v>0.3134</v>
       </c>
       <c r="AX56">
         <v>0.5563</v>
@@ -10454,13 +10454,13 @@
         <v>0.2602</v>
       </c>
       <c r="S57">
-        <v>0.4416</v>
+        <v>0.4393</v>
       </c>
       <c r="T57">
         <v>0.4452</v>
       </c>
       <c r="U57">
-        <v>0.7029</v>
+        <v>0.6615</v>
       </c>
       <c r="V57">
         <v>0.4224</v>
@@ -10472,7 +10472,7 @@
         <v>0.0351</v>
       </c>
       <c r="Y57">
-        <v>0.0344</v>
+        <v>0.0339</v>
       </c>
       <c r="Z57">
         <v>0.1572</v>
@@ -10544,7 +10544,7 @@
         <v>0.0834</v>
       </c>
       <c r="AW57">
-        <v>0.2412</v>
+        <v>0.2128</v>
       </c>
       <c r="AX57">
         <v>0.0002</v>

</xml_diff>